<commit_message>
partial implementation for seeding
</commit_message>
<xml_diff>
--- a/package/Tests/test_validate_data_prerequisites.xlsx
+++ b/package/Tests/test_validate_data_prerequisites.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
   <si>
     <t>Priority</t>
   </si>
@@ -1170,6 +1170,9 @@
   </si>
   <si>
     <t>Prerequisites</t>
+  </si>
+  <si>
+    <t>1,2,3,1,2</t>
   </si>
 </sst>
 </file>
@@ -2208,7 +2211,7 @@
   <dimension ref="B1:Z17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -3034,7 +3037,9 @@
       <c r="S13" s="71">
         <v>1</v>
       </c>
-      <c r="T13" s="73"/>
+      <c r="T13" s="73" t="s">
+        <v>77</v>
+      </c>
       <c r="U13" s="15"/>
       <c r="V13" s="15"/>
       <c r="W13" s="15"/>
@@ -3097,9 +3102,7 @@
         <f t="shared" si="5"/>
         <v>19.833333333333332</v>
       </c>
-      <c r="R14" s="18" t="s">
-        <v>72</v>
-      </c>
+      <c r="R14" s="18"/>
       <c r="S14" s="71">
         <v>1</v>
       </c>

</xml_diff>